<commit_message>
Done with solar light experiment!
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Light_experiment_11-10.xlsx
+++ b/Code/Python/Experiments/Light_experiment_11-10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chineese panel 50x50" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
   <si>
     <t xml:space="preserve">Lamp 60 W halogeen</t>
   </si>
@@ -130,12 +130,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,17 +162,17 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,8 +265,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">0.3719+1.332</f>
-        <v>1.7039</v>
+        <v>1.332</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.357</v>
@@ -319,6 +322,9 @@
       <c r="D14" s="0" t="n">
         <v>17.64</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <v>1179</v>
+      </c>
       <c r="F14" s="0" t="n">
         <v>23</v>
       </c>
@@ -493,11 +499,41 @@
       <c r="A32" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <v>9.276</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>9.615</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>9.496</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>821</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1.803</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2.048</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -511,6 +547,9 @@
       </c>
       <c r="D34" s="0" t="n">
         <v>0.74</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>10550</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>66</v>
@@ -547,13 +586,17 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,16 +604,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>1</v>
@@ -589,15 +622,42 @@
       <c r="A5" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B5" s="2" t="n">
+        <v>66.29</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52.61</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>67.66</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>19.02</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3.738</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>4.021</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>4.114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,16 +670,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>1</v>
@@ -638,15 +688,42 @@
       <c r="A14" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>19.33</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>19.72</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>17.15</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>19.98</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>18.25</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1.385</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1.408</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.357</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,16 +736,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>1</v>
@@ -696,6 +763,15 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.5054</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2.183</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>4.876</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,13 +846,14 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,15 +889,42 @@
       <c r="A5" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>52.07</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>53.84</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>54.09</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>11.25</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>11.73</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2.836</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2.749</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2.846</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,15 +965,42 @@
       <c r="A14" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <v>11.82</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>12.24</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>4.055</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>4.049</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>4.265</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1.616</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1.615</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,15 +1041,42 @@
       <c r="A23" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B23" s="0" t="n">
+        <v>22.36</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>24.74</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B24" s="0" t="n">
+        <v>9.602</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>10.07</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>9.958</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.7703</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.7737</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.7738</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,15 +1117,42 @@
       <c r="A32" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <v>46.53</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>47.63</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>46.71</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>10.09</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1.605</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1.858</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1.852</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update light experiment data from digikey panel (in parallel now)
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Light_experiment_11-10.xlsx
+++ b/Code/Python/Experiments/Light_experiment_11-10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chineese panel 50x50" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <t xml:space="preserve">Lamp 60 W halogeen</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Current temp: no light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLD</t>
   </si>
   <si>
     <t xml:space="preserve">n</t>
@@ -161,9 +164,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,19 +540,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,13 +577,13 @@
         <v>50</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>66.29</v>
+        <v>50.1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>52.61</v>
+        <v>49.75</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>67.66</v>
+        <v>49.24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,13 +591,13 @@
         <v>30</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>15.91</v>
+        <v>8.585</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>19.15</v>
+        <v>9.008</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>19.02</v>
+        <v>8.684</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,13 +605,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>3.738</v>
+        <v>2.764</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>4.021</v>
+        <v>2.756</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>4.114</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,13 +638,13 @@
         <v>50</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>21.2</v>
+        <v>17.05</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>19.33</v>
+        <v>17.13</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>19.72</v>
+        <v>16.81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,13 +652,13 @@
         <v>30</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>17.15</v>
+        <v>6.137</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>19.98</v>
+        <v>6.177</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>18.25</v>
+        <v>6.328</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,13 +666,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1.385</v>
+        <v>0.8086</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1.408</v>
+        <v>0.8198</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1.357</v>
+        <v>0.8358</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,24 +698,42 @@
       <c r="A15" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>10.15</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B16" s="0" t="n">
+        <v>2.947</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2.923</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2.89</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.5054</v>
+        <v>0.4943</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>2.183</v>
+        <v>0.512</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>4.876</v>
+        <v>0.5132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,14 +759,245 @@
       <c r="A21" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B21" s="0" t="n">
+        <v>7.815</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>7.712</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>7.368</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B22" s="0" t="n">
+        <v>1.648</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1.613</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1.635</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.5793</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.5637</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.5474</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>66.29</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>52.61</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>67.66</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3.738</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>4.021</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>4.114</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>19.33</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>19.72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>17.15</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>19.98</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>18.25</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1.385</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1.408</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1.357</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.5054</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2.183</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>4.876</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -767,14 +1019,13 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1272,7 @@
         <v>1.852</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update light experiment data
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Light_experiment_11-10.xlsx
+++ b/Code/Python/Experiments/Light_experiment_11-10.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t xml:space="preserve">Lamp 60 W halogeen</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Current temp: no light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg</t>
   </si>
   <si>
     <t xml:space="preserve">OLD</t>
@@ -164,11 +167,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,17 +543,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,6 +576,9 @@
       <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -585,6 +593,10 @@
       <c r="D3" s="0" t="n">
         <v>49.24</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">(B3+C3+D3)/3</f>
+        <v>49.6966666666667</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -599,6 +611,10 @@
       <c r="D4" s="0" t="n">
         <v>8.684</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">(B4+C4+D4)/3</f>
+        <v>8.759</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -612,6 +628,10 @@
       </c>
       <c r="D5" s="0" t="n">
         <v>2.75</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">(B5+C5+D5)/3</f>
+        <v>2.75666666666667</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,6 +652,9 @@
       <c r="D8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -646,6 +669,10 @@
       <c r="D9" s="0" t="n">
         <v>16.81</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">(B9+C9+D9)/3</f>
+        <v>16.9966666666667</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -660,6 +687,10 @@
       <c r="D10" s="0" t="n">
         <v>6.328</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">(B10+C10+D10)/3</f>
+        <v>6.214</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -673,6 +704,10 @@
       </c>
       <c r="D11" s="0" t="n">
         <v>0.8358</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">(B11+C11+D11)/3</f>
+        <v>0.8214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,6 +728,9 @@
       <c r="D14" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -707,6 +745,10 @@
       <c r="D15" s="0" t="n">
         <v>10.15</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">(B15+C15+D15)/3</f>
+        <v>10.1533333333333</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -721,6 +763,10 @@
       <c r="D16" s="0" t="n">
         <v>2.89</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">(B16+C16+D16)/3</f>
+        <v>2.92</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -734,6 +780,10 @@
       </c>
       <c r="D17" s="0" t="n">
         <v>0.5132</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">(B17+C17+D17)/3</f>
+        <v>0.5065</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,6 +804,9 @@
       <c r="D20" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E20" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -768,6 +821,10 @@
       <c r="D21" s="0" t="n">
         <v>7.368</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">(B21+C21+D21)/3</f>
+        <v>7.63166666666667</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -782,6 +839,10 @@
       <c r="D22" s="0" t="n">
         <v>1.635</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">(B22+C22+D22)/3</f>
+        <v>1.632</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -796,10 +857,14 @@
       <c r="D23" s="0" t="n">
         <v>0.5474</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">(B23+C23+D23)/3</f>
+        <v>0.563466666666667</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,12 +1085,15 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,6 +1114,9 @@
       <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1060,6 +1131,10 @@
       <c r="D3" s="0" t="n">
         <v>54.09</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">(B3+C3+D3)/3</f>
+        <v>53.3333333333333</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1074,6 +1149,10 @@
       <c r="D4" s="0" t="n">
         <v>11.73</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">(B4+C4+D4)/3</f>
+        <v>11.5266666666667</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1087,6 +1166,10 @@
       </c>
       <c r="D5" s="0" t="n">
         <v>2.846</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">(B5+C5+D5)/3</f>
+        <v>2.81033333333333</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,6 +1190,9 @@
       <c r="D8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1121,6 +1207,10 @@
       <c r="D9" s="0" t="n">
         <v>12.24</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">(B9+C9+D9)/3</f>
+        <v>12.09</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1135,6 +1225,10 @@
       <c r="D10" s="0" t="n">
         <v>4.265</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">(B10+C10+D10)/3</f>
+        <v>4.123</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1148,6 +1242,10 @@
       </c>
       <c r="D11" s="0" t="n">
         <v>1.6</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">(B11+C11+D11)/3</f>
+        <v>1.61033333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,6 +1266,9 @@
       <c r="D14" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1182,6 +1283,10 @@
       <c r="D15" s="0" t="n">
         <v>24.74</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">(B15+C15+D15)/3</f>
+        <v>23.1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1196,6 +1301,10 @@
       <c r="D16" s="0" t="n">
         <v>9.958</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">(B16+C16+D16)/3</f>
+        <v>9.87666666666667</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1209,6 +1318,10 @@
       </c>
       <c r="D17" s="0" t="n">
         <v>0.7738</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">(B17+C17+D17)/3</f>
+        <v>0.7726</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,6 +1342,9 @@
       <c r="D20" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E20" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1243,6 +1359,10 @@
       <c r="D21" s="0" t="n">
         <v>46.71</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">(B21+C21+D21)/3</f>
+        <v>46.9566666666667</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1257,6 +1377,10 @@
       <c r="D22" s="0" t="n">
         <v>10.09</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">(B22+C22+D22)/3</f>
+        <v>10.1633333333333</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1271,8 +1395,12 @@
       <c r="D23" s="0" t="n">
         <v>1.852</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">(B23+C23+D23)/3</f>
+        <v>1.77166666666667</v>
+      </c>
       <c r="M23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>